<commit_message>
db khdamna awal test khasna fih ghi buttons
</commit_message>
<xml_diff>
--- a/liste tests.xlsx
+++ b/liste tests.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374FD18E-D38B-4EF4-A99A-D0E7CD5357E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE102D8-71A9-4BC4-A892-5822FB63F62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
   <si>
     <t>Telehealth Patient Checklist</t>
   </si>
@@ -243,13 +245,485 @@
   </si>
   <si>
     <t>q10</t>
+  </si>
+  <si>
+    <t>رقم السؤال في الاختبار العام</t>
+  </si>
+  <si>
+    <t>موضوع السؤال</t>
+  </si>
+  <si>
+    <t>الاختبارات التي يجب اقتراحها عند ارتفاع الدرجة</t>
+  </si>
+  <si>
+    <t>1 — القلق العام</t>
+  </si>
+  <si>
+    <t>شعور عام بالقلق والتوتر</t>
+  </si>
+  <si>
+    <t>GAD‑7</t>
+  </si>
+  <si>
+    <t>2 — الحزن وفقدان المتعة</t>
+  </si>
+  <si>
+    <t>أعراض اكتئابية مزاجية</t>
+  </si>
+  <si>
+    <t>PHQ‑9</t>
+  </si>
+  <si>
+    <t>3 — مشاكل النوم</t>
+  </si>
+  <si>
+    <t>أرق وصعوبات نوم</t>
+  </si>
+  <si>
+    <r>
+      <t>ISI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + أحيانًا </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHQ‑9</t>
+    </r>
+  </si>
+  <si>
+    <t>4 — استرجاع أحداث صادمة</t>
+  </si>
+  <si>
+    <t>ذكريات/كوابيس/Flashbacks</t>
+  </si>
+  <si>
+    <t>PCL‑5</t>
+  </si>
+  <si>
+    <t>5 — التجنب والانسحاب</t>
+  </si>
+  <si>
+    <t>تجنب محفزات الصدمة أو العزلة</t>
+  </si>
+  <si>
+    <r>
+      <t>PCL‑5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHQ‑9</t>
+    </r>
+  </si>
+  <si>
+    <t>6 — الذنب/لوم الذات</t>
+  </si>
+  <si>
+    <t>تفكير سلبي ولوم الذات</t>
+  </si>
+  <si>
+    <r>
+      <t>PHQ‑9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PCL‑5</t>
+    </r>
+  </si>
+  <si>
+    <t>7 — أعراض جسدية مرتبطة بالقلق</t>
+  </si>
+  <si>
+    <t>ردود فعل جسدية للتوتر</t>
+  </si>
+  <si>
+    <r>
+      <t>GAD‑7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + قد يرتبط بـ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PCL‑5</t>
+    </r>
+  </si>
+  <si>
+    <t>8 — صعوبة التركيز والانتباه</t>
+  </si>
+  <si>
+    <t>تشتت ذهني وعجز معرفي</t>
+  </si>
+  <si>
+    <r>
+      <t>PHQ‑9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PCL‑5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GAD‑7</t>
+    </r>
+  </si>
+  <si>
+    <t>9 — استخدام الكحول/المخدرات</t>
+  </si>
+  <si>
+    <t>سلوك تعاطي أو إساءة استخدام</t>
+  </si>
+  <si>
+    <r>
+      <t>AUDIT‑C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AUDIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DAST‑10</t>
+    </r>
+  </si>
+  <si>
+    <t>10 — الاندفاع والسلوكيات الخطرة</t>
+  </si>
+  <si>
+    <t>سلوك خطير أو متهور</t>
+  </si>
+  <si>
+    <r>
+      <t>PCL‑5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DAST‑10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AUDIT</t>
+    </r>
+  </si>
+  <si>
+    <t>11 — (JOKER) أفكار إيذاء النفس/الانتحار</t>
+  </si>
+  <si>
+    <t>خطر حاد على الذات</t>
+  </si>
+  <si>
+    <r>
+      <t>C‑SSRS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (فوري) + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHQ‑9 (سؤال 9)</t>
+    </r>
+  </si>
+  <si>
+    <t>ISI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUDIT‑C </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AUDIT</t>
+  </si>
+  <si>
+    <t>DAST‑10</t>
+  </si>
+  <si>
+    <t>C‑SSRS</t>
+  </si>
+  <si>
+    <t>q1,7,8</t>
+  </si>
+  <si>
+    <t>q2,3,5,6,8,11</t>
+  </si>
+  <si>
+    <t>q4,5,6,7,8,10</t>
+  </si>
+  <si>
+    <t>q9,10</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بعد الاجابة على كل الاسئلة و تحديد الاجابات نشغل سيناريو السؤال 11 اذا نعم نوجهه ل C‑SSRS مباشرة اذا ا لا نعرض رسالة و نقارن من سيضهر مثال اعرض PHQ‑9 </t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>PHQ9_Score</t>
+  </si>
+  <si>
+    <t>GAD7_Score</t>
+  </si>
+  <si>
+    <t>PCL5_Score</t>
+  </si>
+  <si>
+    <t>ISI_Score</t>
+  </si>
+  <si>
+    <t>AUDIT_C_Score</t>
+  </si>
+  <si>
+    <t>AUDIT_Score</t>
+  </si>
+  <si>
+    <t>DAST10_Score</t>
+  </si>
+  <si>
+    <t>Display_PHQ9</t>
+  </si>
+  <si>
+    <t>Display_GAD7</t>
+  </si>
+  <si>
+    <t>Display_PCL5</t>
+  </si>
+  <si>
+    <t>Display_ISI</t>
+  </si>
+  <si>
+    <t>Display_AUDIT_C</t>
+  </si>
+  <si>
+    <t>Display_AUDIT</t>
+  </si>
+  <si>
+    <t>Display_DAST10</t>
+  </si>
+  <si>
+    <t>Suicide_Level</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>نظام الإجابة المقترح لكل سؤال: 0 = أبدًا  1 = قليلًا  2 = أحيانًا  3 = غالبًا  4 = دائمًا قلق عام: أشعر بالقلق أو التوتر في أغلب الأيام دون سبب واضح أو بسبب عدة أمور. الحزن وفقدان المتعة: أشعر بحزن، إحباط، أو فقدان رغبة في القيام بالأشياء التي كانت تسعدني. مشاكل النوم: أعاني من صعوبة في النوم أو الاستيقاظ المتكرر أو النوم المفرط. استرجاع أحداث مؤلمة: تراودني ذكريات أو أحلام مزعجة مرتبطة بتجارب صعبة مررت بها. تجنب أو انسحاب اجتماعي: أتجنب الناس أو الأماكن أو الأنشطة بسبب مشاعر داخلية مزعجة. مشاعر الذنب أو لوم الذات: أشعر أنني مخطئ أو مذنب أو ألوم نفسي بشكل متكرر. أعراض جسدية مرتبطة بالتوتر: أشعر بتسارع ضربات القلب، ضيق تنفس، ارتجاف، تعرق، أو توتر جسدي. صعوبة التركيز: أواجه صعوبة في التركيز، التذكر، أو متابعة المهام اليومية. استخدام مواد نفسية (كحول/مخدرات): أستخدم الكحول أو مواد أخرى بشكل قد يؤثر على حياتي أو علاقتي بالآخرين. اندفاع أو سلوكيات خطرة: أقوم أحيانًا بسلوكيات خطرة أو اندفاعية (مثل قيادة متهورة، صرف مفرط، شجارات، إيذاء غير مقصود) دون تفكير في العواقب.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +759,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -300,7 +781,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -349,12 +830,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -375,11 +865,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -665,7 +1169,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,7 +1324,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -877,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65CA5F2-15D5-4B3B-90F7-F490FFC3DC0B}">
   <dimension ref="F1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1256,4 +1760,361 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD2F276-4C6A-4482-9F66-8A4C148A13DE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4E7752-649E-4DA3-BBC9-6991F93C44A2}">
+  <dimension ref="A1:AD14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="D14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="U14" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="X14" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y14" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA14" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB14" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD14" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>